<commit_message>
versao com correcao de
</commit_message>
<xml_diff>
--- a/BalanceUs - Resumo.xlsx
+++ b/BalanceUs - Resumo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="55">
   <si>
     <t>Resumo dos Dados</t>
   </si>
@@ -104,28 +104,55 @@
     <t>Unimed</t>
   </si>
   <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>15918,74</t>
-  </si>
-  <si>
-    <t>1299,77</t>
-  </si>
-  <si>
-    <t>303</t>
-  </si>
-  <si>
-    <t>25330,08</t>
-  </si>
-  <si>
-    <t>2319,65</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>1362,81</t>
+    <t>219</t>
+  </si>
+  <si>
+    <t>17278,13</t>
+  </si>
+  <si>
+    <t>1411,06</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>25514,24</t>
+  </si>
+  <si>
+    <t>2340,26</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>1570,61</t>
+  </si>
+  <si>
+    <t>Unimed PF</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>5994,24</t>
+  </si>
+  <si>
+    <t>458,68</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>5083,59</t>
+  </si>
+  <si>
+    <t>407,75</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>128,38</t>
   </si>
   <si>
     <t/>
@@ -134,16 +161,22 @@
     <t>Geral</t>
   </si>
   <si>
-    <t>210</t>
-  </si>
-  <si>
-    <t>16864,77</t>
-  </si>
-  <si>
-    <t>317</t>
-  </si>
-  <si>
-    <t>27305,15</t>
+    <t>294</t>
+  </si>
+  <si>
+    <t>35502,29</t>
+  </si>
+  <si>
+    <t>377</t>
+  </si>
+  <si>
+    <t>53003,55</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>3141,22</t>
   </si>
 </sst>
 </file>
@@ -201,7 +234,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -649,33 +682,42 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
         <v>38</v>
-      </c>
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>39</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
       <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" t="s">
         <v>40</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>41</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
         <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" t="s">
-        <v>39</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
@@ -686,16 +728,25 @@
       <c r="F24" t="s">
         <v>15</v>
       </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
         <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -706,25 +757,114 @@
       <c r="F25" t="s">
         <v>43</v>
       </c>
+      <c r="G25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
         <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" t="s">
-        <v>39</v>
       </c>
       <c r="D26" t="s">
         <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>